<commit_message>
updated filter system for binder, turn on filters D-H
</commit_message>
<xml_diff>
--- a/ABSOLUTE SIZE data/concepts from binder.xlsx
+++ b/ABSOLUTE SIZE data/concepts from binder.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaritapopova/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaritapopova/Desktop/size matters/SizeMatters/ABSOLUTE SIZE data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EAA36D8-7BD1-724E-8DF9-E85FD14C1879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982EB018-CE0E-D74C-998E-05CE9050DFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="4000" windowWidth="25240" windowHeight="12680" xr2:uid="{2C4F6887-E128-2A46-B4B8-C730199AF56F}"/>
+    <workbookView xWindow="1440" yWindow="500" windowWidth="26260" windowHeight="14480" xr2:uid="{2C4F6887-E128-2A46-B4B8-C730199AF56F}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$I$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="231">
   <si>
     <t>zoo</t>
   </si>
@@ -707,16 +710,53 @@
   </si>
   <si>
     <t>Word</t>
+  </si>
+  <si>
+    <t>abstracts?</t>
+  </si>
+  <si>
+    <t>masses?</t>
+  </si>
+  <si>
+    <t>useless?</t>
+  </si>
+  <si>
+    <t>singulatives?</t>
+  </si>
+  <si>
+    <t>veggies?</t>
+  </si>
+  <si>
+    <t>suspicious?</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -742,8 +782,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1058,27 +1100,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BE3EEF-2A4D-5842-A234-ED0216293D76}">
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:I222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>220</v>
       </c>
@@ -1088,8 +1148,11 @@
       <c r="C2">
         <v>1.137931</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>219</v>
       </c>
@@ -1099,8 +1162,11 @@
       <c r="C3">
         <v>0.71428599999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>218</v>
       </c>
@@ -1110,8 +1176,11 @@
       <c r="C4">
         <v>0.137931</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -1121,8 +1190,11 @@
       <c r="C5">
         <v>0.43333300000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>216</v>
       </c>
@@ -1132,8 +1204,11 @@
       <c r="C6">
         <v>0.25806499999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>215</v>
       </c>
@@ -1144,7 +1219,7 @@
         <v>5.8709680000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -1155,7 +1230,7 @@
         <v>0.96428599999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -1165,8 +1240,11 @@
       <c r="C9">
         <v>4.4333330000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>212</v>
       </c>
@@ -1177,7 +1255,7 @@
         <v>1.4666669999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>211</v>
       </c>
@@ -1187,8 +1265,14 @@
       <c r="C11">
         <v>3.5172409999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>210</v>
       </c>
@@ -1199,7 +1283,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>209</v>
       </c>
@@ -1209,8 +1293,11 @@
       <c r="C13">
         <v>1.321429</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -1221,7 +1308,7 @@
         <v>3.4074070000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>207</v>
       </c>
@@ -1231,8 +1318,14 @@
       <c r="C15">
         <v>3.2758620000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>230</v>
+      </c>
+      <c r="I15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>206</v>
       </c>
@@ -1242,8 +1335,11 @@
       <c r="C16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>205</v>
       </c>
@@ -1253,8 +1349,11 @@
       <c r="C17">
         <v>0.85714299999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>204</v>
       </c>
@@ -1264,8 +1363,11 @@
       <c r="C18">
         <v>4.6071429999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>203</v>
       </c>
@@ -1275,8 +1377,11 @@
       <c r="C19">
         <v>0.24137900000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>202</v>
       </c>
@@ -1286,8 +1391,11 @@
       <c r="C20">
         <v>0.17241400000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>201</v>
       </c>
@@ -1298,7 +1406,7 @@
         <v>0.73333300000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -1309,7 +1417,7 @@
         <v>5.0967739999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>199</v>
       </c>
@@ -1319,8 +1427,11 @@
       <c r="C23">
         <v>2.233333</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>198</v>
       </c>
@@ -1331,7 +1442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -1341,8 +1452,11 @@
       <c r="C25">
         <v>1.266667</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -1353,7 +1467,7 @@
         <v>4.0344829999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>195</v>
       </c>
@@ -1363,8 +1477,11 @@
       <c r="C27">
         <v>5.5862069999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>194</v>
       </c>
@@ -1375,7 +1492,7 @@
         <v>0.71428599999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>193</v>
       </c>
@@ -1386,7 +1503,7 @@
         <v>2.8666670000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -1396,8 +1513,11 @@
       <c r="C30">
         <v>2.9032260000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -1408,7 +1528,7 @@
         <v>0.34482800000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>190</v>
       </c>
@@ -1418,8 +1538,14 @@
       <c r="C32">
         <v>3.8333330000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>230</v>
+      </c>
+      <c r="H32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>189</v>
       </c>
@@ -1430,7 +1556,7 @@
         <v>1.964286</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -1440,8 +1566,11 @@
       <c r="C34">
         <v>0.17857100000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>187</v>
       </c>
@@ -1452,7 +1581,7 @@
         <v>5.1333330000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>186</v>
       </c>
@@ -1463,7 +1592,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>185</v>
       </c>
@@ -1473,8 +1602,11 @@
       <c r="C37">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>184</v>
       </c>
@@ -1484,8 +1616,11 @@
       <c r="C38">
         <v>1.65625</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>183</v>
       </c>
@@ -1495,8 +1630,11 @@
       <c r="C39">
         <v>0.43333300000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>182</v>
       </c>
@@ -1507,7 +1645,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -1517,8 +1655,11 @@
       <c r="C41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>180</v>
       </c>
@@ -1529,7 +1670,7 @@
         <v>0.206897</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -1540,7 +1681,7 @@
         <v>0.275862</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>178</v>
       </c>
@@ -1550,8 +1691,11 @@
       <c r="C44">
         <v>3.2758620000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -1561,8 +1705,11 @@
       <c r="C45">
         <v>3.6428569999999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>176</v>
       </c>
@@ -1572,8 +1719,11 @@
       <c r="C46">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>175</v>
       </c>
@@ -1583,8 +1733,11 @@
       <c r="C47">
         <v>4.7419349999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -1595,7 +1748,7 @@
         <v>1.6538459999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>173</v>
       </c>
@@ -1605,8 +1758,11 @@
       <c r="C49">
         <v>3.266667</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>172</v>
       </c>
@@ -1616,8 +1772,11 @@
       <c r="C50">
         <v>0.96551699999999996</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>171</v>
       </c>
@@ -1627,8 +1786,11 @@
       <c r="C51">
         <v>5.3333329999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>170</v>
       </c>
@@ -1638,8 +1800,11 @@
       <c r="C52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -1650,7 +1815,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>168</v>
       </c>
@@ -1660,8 +1825,11 @@
       <c r="C54">
         <v>2.5666669999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>167</v>
       </c>
@@ -1671,8 +1839,11 @@
       <c r="C55">
         <v>4.233333</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>166</v>
       </c>
@@ -1683,7 +1854,7 @@
         <v>3.4827590000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>165</v>
       </c>
@@ -1694,7 +1865,7 @@
         <v>0.30769200000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>164</v>
       </c>
@@ -1704,8 +1875,11 @@
       <c r="C58">
         <v>2.9032260000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>163</v>
       </c>
@@ -1716,7 +1890,7 @@
         <v>0.26666699999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>162</v>
       </c>
@@ -1726,8 +1900,11 @@
       <c r="C60">
         <v>2.4375</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>161</v>
       </c>
@@ -1737,8 +1914,11 @@
       <c r="C61">
         <v>0.58620700000000003</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I61" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>160</v>
       </c>
@@ -1749,7 +1929,7 @@
         <v>4.1612900000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>159</v>
       </c>
@@ -1760,7 +1940,7 @@
         <v>3.8666670000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>158</v>
       </c>
@@ -1770,8 +1950,11 @@
       <c r="C64">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>157</v>
       </c>
@@ -1781,8 +1964,11 @@
       <c r="C65">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>156</v>
       </c>
@@ -1792,8 +1978,11 @@
       <c r="C66">
         <v>5.2068969999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>155</v>
       </c>
@@ -1804,7 +1993,7 @@
         <v>0.96428599999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -1815,7 +2004,7 @@
         <v>3.0689660000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -1825,8 +2014,11 @@
       <c r="C69">
         <v>2.7096770000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>152</v>
       </c>
@@ -1837,7 +2029,7 @@
         <v>4.4827589999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>151</v>
       </c>
@@ -1848,7 +2040,7 @@
         <v>0.74193500000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>150</v>
       </c>
@@ -1859,7 +2051,7 @@
         <v>5.2857139999999996</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -1870,7 +2062,7 @@
         <v>2.4193549999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -1880,8 +2072,11 @@
       <c r="C74">
         <v>0.63333300000000003</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>147</v>
       </c>
@@ -1892,7 +2087,7 @@
         <v>0.89285700000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>146</v>
       </c>
@@ -1902,8 +2097,11 @@
       <c r="C76">
         <v>1.4193549999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -1914,7 +2112,7 @@
         <v>3.3928569999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>144</v>
       </c>
@@ -1925,7 +2123,7 @@
         <v>4.9354839999999998</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -1935,8 +2133,11 @@
       <c r="C79">
         <v>2.8965519999999998</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>142</v>
       </c>
@@ -1947,7 +2148,7 @@
         <v>0.12903200000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>141</v>
       </c>
@@ -1957,8 +2158,11 @@
       <c r="C81">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I81" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -1968,8 +2172,11 @@
       <c r="C82">
         <v>0.44444400000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I82" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>139</v>
       </c>
@@ -1979,8 +2186,11 @@
       <c r="C83">
         <v>0.34615400000000002</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I83" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>138</v>
       </c>
@@ -1990,8 +2200,11 @@
       <c r="C84">
         <v>0.26666699999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F84" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>137</v>
       </c>
@@ -2002,7 +2215,7 @@
         <v>4.5666669999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>136</v>
       </c>
@@ -2012,8 +2225,11 @@
       <c r="C86">
         <v>0.12903200000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I86" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>135</v>
       </c>
@@ -2023,8 +2239,11 @@
       <c r="C87">
         <v>2.4666670000000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I87" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>134</v>
       </c>
@@ -2035,7 +2254,7 @@
         <v>4.3448279999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>133</v>
       </c>
@@ -2046,7 +2265,7 @@
         <v>0.65517199999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>132</v>
       </c>
@@ -2056,8 +2275,11 @@
       <c r="C90">
         <v>2.714286</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F90" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -2068,7 +2290,7 @@
         <v>0.62068999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>130</v>
       </c>
@@ -2079,7 +2301,7 @@
         <v>3.2413789999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>129</v>
       </c>
@@ -2090,7 +2312,7 @@
         <v>3.1428569999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>128</v>
       </c>
@@ -2101,7 +2323,7 @@
         <v>4.2903229999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>127</v>
       </c>
@@ -2112,7 +2334,7 @@
         <v>3.0689660000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>126</v>
       </c>
@@ -2123,7 +2345,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>125</v>
       </c>
@@ -2133,8 +2355,11 @@
       <c r="C97">
         <v>2.535714</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F97" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>124</v>
       </c>
@@ -2145,7 +2370,7 @@
         <v>7.1429000000000006E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>123</v>
       </c>
@@ -2155,8 +2380,11 @@
       <c r="C99">
         <v>1.035714</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I99" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>122</v>
       </c>
@@ -2167,7 +2395,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>121</v>
       </c>
@@ -2178,7 +2406,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -2188,8 +2416,11 @@
       <c r="C102">
         <v>5.1875</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I102" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -2199,8 +2430,11 @@
       <c r="C103">
         <v>0.793103</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F103" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -2211,7 +2445,7 @@
         <v>4.9285709999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>117</v>
       </c>
@@ -2221,8 +2455,14 @@
       <c r="C105">
         <v>2.3793099999999998</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E105" t="s">
+        <v>230</v>
+      </c>
+      <c r="G105" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>116</v>
       </c>
@@ -2233,7 +2473,7 @@
         <v>3.3333330000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>115</v>
       </c>
@@ -2244,7 +2484,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -2254,8 +2494,11 @@
       <c r="C108">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E108" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -2265,8 +2508,11 @@
       <c r="C109">
         <v>5.0344829999999998</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I109" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -2277,7 +2523,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -2287,8 +2533,11 @@
       <c r="C111">
         <v>4.3103449999999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F111" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2298,8 +2547,11 @@
       <c r="C112">
         <v>0.793103</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F112" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -2310,7 +2562,7 @@
         <v>2.3870969999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>108</v>
       </c>
@@ -2320,8 +2572,11 @@
       <c r="C114">
         <v>0.12903200000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I114" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>107</v>
       </c>
@@ -2332,7 +2587,7 @@
         <v>1.2068970000000001</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>106</v>
       </c>
@@ -2343,7 +2598,7 @@
         <v>0.44827600000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>105</v>
       </c>
@@ -2353,8 +2608,11 @@
       <c r="C117">
         <v>2.285714</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E117" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -2365,7 +2623,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>103</v>
       </c>
@@ -2376,7 +2634,7 @@
         <v>0.25806499999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>102</v>
       </c>
@@ -2386,8 +2644,11 @@
       <c r="C120">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I120" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>101</v>
       </c>
@@ -2397,8 +2658,11 @@
       <c r="C121">
         <v>2.964286</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E121" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -2409,7 +2673,7 @@
         <v>0.83333299999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>99</v>
       </c>
@@ -2420,7 +2684,7 @@
         <v>1.8666670000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>98</v>
       </c>
@@ -2430,8 +2694,11 @@
       <c r="C124">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E124" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>97</v>
       </c>
@@ -2442,7 +2709,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>96</v>
       </c>
@@ -2452,8 +2719,11 @@
       <c r="C126">
         <v>0.17241400000000001</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I126" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>95</v>
       </c>
@@ -2463,8 +2733,11 @@
       <c r="C127">
         <v>2.3103449999999999</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F127" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>94</v>
       </c>
@@ -2475,7 +2748,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>93</v>
       </c>
@@ -2485,8 +2758,11 @@
       <c r="C129">
         <v>2.137931</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I129" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>92</v>
       </c>
@@ -2497,7 +2773,7 @@
         <v>0.96551699999999996</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>91</v>
       </c>
@@ -2507,8 +2783,11 @@
       <c r="C131">
         <v>0.48275899999999999</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I131" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>90</v>
       </c>
@@ -2519,7 +2798,7 @@
         <v>0.55172399999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>89</v>
       </c>
@@ -2530,7 +2809,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>88</v>
       </c>
@@ -2540,8 +2819,11 @@
       <c r="C134">
         <v>2.3333330000000001</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E134" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>87</v>
       </c>
@@ -2551,8 +2833,11 @@
       <c r="C135">
         <v>7.1429000000000006E-2</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F135" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>86</v>
       </c>
@@ -2563,7 +2848,7 @@
         <v>3.7241379999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>85</v>
       </c>
@@ -2574,7 +2859,7 @@
         <v>3.4482759999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>84</v>
       </c>
@@ -2584,8 +2869,11 @@
       <c r="C138">
         <v>2.1666669999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F138" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>83</v>
       </c>
@@ -2596,7 +2884,7 @@
         <v>4.4827589999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>82</v>
       </c>
@@ -2606,8 +2894,11 @@
       <c r="C140">
         <v>2.0333329999999998</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I140" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>81</v>
       </c>
@@ -2618,7 +2909,7 @@
         <v>2.1481479999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>80</v>
       </c>
@@ -2629,7 +2920,7 @@
         <v>0.24137900000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>79</v>
       </c>
@@ -2640,7 +2931,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>78</v>
       </c>
@@ -2651,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>77</v>
       </c>
@@ -2662,7 +2953,7 @@
         <v>5.4375</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>76</v>
       </c>
@@ -2673,7 +2964,7 @@
         <v>3.6428569999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>75</v>
       </c>
@@ -2684,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>74</v>
       </c>
@@ -2695,7 +2986,7 @@
         <v>4.7931030000000003</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>73</v>
       </c>
@@ -2705,8 +2996,11 @@
       <c r="C149">
         <v>2.8666670000000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E149" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>72</v>
       </c>
@@ -2717,7 +3011,7 @@
         <v>2.5666669999999998</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>71</v>
       </c>
@@ -2728,7 +3022,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>70</v>
       </c>
@@ -2739,7 +3033,7 @@
         <v>0.40740700000000002</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>69</v>
       </c>
@@ -2749,8 +3043,11 @@
       <c r="C153">
         <v>0.57142899999999996</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F153" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>68</v>
       </c>
@@ -2761,7 +3058,7 @@
         <v>2.461538</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>67</v>
       </c>
@@ -2772,7 +3069,7 @@
         <v>0.56666700000000003</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>66</v>
       </c>
@@ -2782,8 +3079,14 @@
       <c r="C156">
         <v>5.6896550000000001</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G156" t="s">
+        <v>230</v>
+      </c>
+      <c r="H156" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>65</v>
       </c>
@@ -2794,7 +3097,7 @@
         <v>4.5862069999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>64</v>
       </c>
@@ -2805,7 +3108,7 @@
         <v>4.6666670000000003</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>63</v>
       </c>
@@ -2815,8 +3118,11 @@
       <c r="C159">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I159" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>62</v>
       </c>
@@ -2826,8 +3132,11 @@
       <c r="C160">
         <v>0.42857099999999998</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I160" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>61</v>
       </c>
@@ -2838,7 +3147,7 @@
         <v>2.535714</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>60</v>
       </c>
@@ -2849,7 +3158,7 @@
         <v>1.433333</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>59</v>
       </c>
@@ -2859,8 +3168,11 @@
       <c r="C163">
         <v>2.4137930000000001</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H163" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>58</v>
       </c>
@@ -2870,8 +3182,11 @@
       <c r="C164">
         <v>0.13333300000000001</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I164" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>57</v>
       </c>
@@ -2881,8 +3196,11 @@
       <c r="C165">
         <v>4.1724139999999998</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H165" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>56</v>
       </c>
@@ -2892,8 +3210,11 @@
       <c r="C166">
         <v>0.41379300000000002</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F166" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>55</v>
       </c>
@@ -2904,7 +3225,7 @@
         <v>0.16666700000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>54</v>
       </c>
@@ -2914,8 +3235,11 @@
       <c r="C168">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H168" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>53</v>
       </c>
@@ -2925,8 +3249,11 @@
       <c r="C169">
         <v>4.3103449999999999</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H169" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>52</v>
       </c>
@@ -2937,7 +3264,7 @@
         <v>1.4074070000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>51</v>
       </c>
@@ -2947,8 +3274,11 @@
       <c r="C171">
         <v>5.2758620000000001</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H171" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>50</v>
       </c>
@@ -2958,8 +3288,11 @@
       <c r="C172">
         <v>0.71428599999999998</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I172" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>49</v>
       </c>
@@ -2970,7 +3303,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -2980,8 +3313,11 @@
       <c r="C174">
         <v>0.23333300000000001</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F174" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -2992,7 +3328,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>46</v>
       </c>
@@ -3002,8 +3338,11 @@
       <c r="C176">
         <v>1.7777780000000001</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E176" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>45</v>
       </c>
@@ -3013,8 +3352,11 @@
       <c r="C177">
         <v>0.77777799999999997</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I177" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>44</v>
       </c>
@@ -3024,8 +3366,11 @@
       <c r="C178">
         <v>2.6129030000000002</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I178" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>43</v>
       </c>
@@ -3035,8 +3380,11 @@
       <c r="C179">
         <v>3.3793099999999998</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E179" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>42</v>
       </c>
@@ -3046,8 +3394,11 @@
       <c r="C180">
         <v>1.3666670000000001</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F180" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>41</v>
       </c>
@@ -3058,7 +3409,7 @@
         <v>0.34615400000000002</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>40</v>
       </c>
@@ -3069,7 +3420,7 @@
         <v>3.5714290000000002</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>39</v>
       </c>
@@ -3079,8 +3430,11 @@
       <c r="C183">
         <v>1.4482759999999999</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F183" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>38</v>
       </c>
@@ -3091,7 +3445,7 @@
         <v>1.4827589999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>37</v>
       </c>
@@ -3102,7 +3456,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>36</v>
       </c>
@@ -3113,7 +3467,7 @@
         <v>1.8064519999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>35</v>
       </c>
@@ -3124,7 +3478,7 @@
         <v>2.548387</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>34</v>
       </c>
@@ -3134,8 +3488,11 @@
       <c r="C188">
         <v>2.6666669999999999</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F188" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>33</v>
       </c>
@@ -3145,8 +3502,11 @@
       <c r="C189">
         <v>2.8666670000000001</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I189" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>32</v>
       </c>
@@ -3156,8 +3516,11 @@
       <c r="C190">
         <v>3.5517240000000001</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F190" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>31</v>
       </c>
@@ -3168,7 +3531,7 @@
         <v>3.1071430000000002</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>30</v>
       </c>
@@ -3179,7 +3542,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>29</v>
       </c>
@@ -3190,7 +3553,7 @@
         <v>0.466667</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>28</v>
       </c>
@@ -3200,8 +3563,11 @@
       <c r="C194">
         <v>7.4074000000000001E-2</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F194" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>27</v>
       </c>
@@ -3211,8 +3577,11 @@
       <c r="C195">
         <v>0.103448</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I195" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>26</v>
       </c>
@@ -3223,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>25</v>
       </c>
@@ -3234,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>24</v>
       </c>
@@ -3244,8 +3613,11 @@
       <c r="C198">
         <v>4.4827589999999997</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H198" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>23</v>
       </c>
@@ -3256,7 +3628,7 @@
         <v>2.233333</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>22</v>
       </c>
@@ -3267,7 +3639,7 @@
         <v>0.20833299999999999</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>21</v>
       </c>
@@ -3278,7 +3650,7 @@
         <v>4.8214290000000002</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>20</v>
       </c>
@@ -3289,7 +3661,7 @@
         <v>0.53571400000000002</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>19</v>
       </c>
@@ -3299,8 +3671,11 @@
       <c r="C203">
         <v>2.9655170000000002</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F203" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>18</v>
       </c>
@@ -3310,8 +3685,11 @@
       <c r="C204">
         <v>3.3666670000000001</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E204" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>17</v>
       </c>
@@ -3322,7 +3700,7 @@
         <v>4.9310340000000004</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -3332,8 +3710,11 @@
       <c r="C206">
         <v>4.0666669999999998</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H206" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>15</v>
       </c>
@@ -3344,7 +3725,7 @@
         <v>6.6667000000000004E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3736,7 @@
         <v>0.38709700000000002</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>13</v>
       </c>
@@ -3365,8 +3746,11 @@
       <c r="C209">
         <v>1.137931</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F209" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>12</v>
       </c>
@@ -3376,8 +3760,11 @@
       <c r="C210">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I210" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -3387,8 +3774,11 @@
       <c r="C211">
         <v>1.8333330000000001</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F211" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>10</v>
       </c>
@@ -3398,8 +3788,11 @@
       <c r="C212">
         <v>0.466667</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F212" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -3410,7 +3803,7 @@
         <v>4.0344829999999998</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>8</v>
       </c>
@@ -3420,8 +3813,11 @@
       <c r="C214">
         <v>3</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I214" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>7</v>
       </c>
@@ -3432,7 +3828,7 @@
         <v>2.0344829999999998</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>6</v>
       </c>
@@ -3442,8 +3838,11 @@
       <c r="C216">
         <v>0.25925900000000002</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I216" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>5</v>
       </c>
@@ -3453,8 +3852,11 @@
       <c r="C217">
         <v>7.1429000000000006E-2</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I217" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>4</v>
       </c>
@@ -3464,8 +3866,11 @@
       <c r="C218">
         <v>0.72413799999999995</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E218" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>3</v>
       </c>
@@ -3475,8 +3880,11 @@
       <c r="C219">
         <v>3.3333000000000002E-2</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I219" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>2</v>
       </c>
@@ -3487,7 +3895,7 @@
         <v>1.392857</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>1</v>
       </c>
@@ -3497,8 +3905,11 @@
       <c r="C221">
         <v>1.5172410000000001</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F221" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -3508,8 +3919,12 @@
       <c r="C222">
         <v>6.6667000000000004E-2</v>
       </c>
+      <c r="I222" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{45BE3EEF-2A4D-5842-A234-ED0216293D76}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>